<commit_message>
added more hybrid models
</commit_message>
<xml_diff>
--- a/models_and_metrics/metrics_summary.xlsx
+++ b/models_and_metrics/metrics_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio Coding\DL_final_project\models_and_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245DC1BC-1F4C-4FA1-A503-F305E5207445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FD3654-2292-454F-ACF7-88B33F563486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32CD13F7-3551-4E15-BA67-D6630EDB706E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32CD13F7-3551-4E15-BA67-D6630EDB706E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,15 +137,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,9 +241,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Base Premade</c:v>
                 </c:pt>
@@ -263,16 +264,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Rotary</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hybrid 1 (Rotary + RMS)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hybrid 2 (Rotary + RMS + GLU)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Hybrid 3 (Rotary + RMS + EA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$8</c:f>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.60298507462686501</c:v>
                 </c:pt>
@@ -293,6 +303,15 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.68656716417910402</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68805970149253703</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70646766169154196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69253731343283498</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -552,9 +571,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Base Premade</c:v>
                 </c:pt>
@@ -575,16 +594,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Rotary</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hybrid 1 (Rotary + RMS)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hybrid 2 (Rotary + RMS + GLU)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Hybrid 3 (Rotary + RMS + EA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.5467571644042233</c:v>
                 </c:pt>
@@ -605,6 +633,15 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.5191614066726782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5224074474994587</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1943788886505042</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3572669368847712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,9 +901,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Base Premade</c:v>
                 </c:pt>
@@ -887,16 +924,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Rotary</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hybrid 1 (Rotary + RMS)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hybrid 2 (Rotary + RMS + GLU)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Hybrid 3 (Rotary + RMS + EA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.7056463190300515</c:v>
                 </c:pt>
@@ -917,6 +963,15 @@
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>2.4855667830802886</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.5262958971993039</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1.999136761053476</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>2.2777102172730075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1176,9 +1231,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Base Premade</c:v>
                 </c:pt>
@@ -1199,16 +1254,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Rotary</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hybrid 1 (Rotary + RMS)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hybrid 2 (Rotary + RMS + GLU)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Hybrid 3 (Rotary + RMS + EA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:f>Sheet1!$J$2:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>85806346</c:v>
                 </c:pt>
@@ -1229,6 +1293,15 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>85653514</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85635082</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113983498</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85635094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3588,15 +3661,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4052,401 +4125,427 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>2652</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>14</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>C2*293/B2</f>
         <v>1.5467571644042233</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <f>32 / 11.8271186351776</f>
         <v>2.7056463190300515</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0.63613738178198098</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>0.60298507462686501</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>0.60112383449298201</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>0.61423096264957999</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>85806346</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>3867</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>21</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D6" si="0">C3*293/B3</f>
         <v>1.5911559348332041</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <f>32 / 11.816104888916</f>
         <v>2.708168241635815</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.67048282727725195</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>0.65124378109452696</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>0.64995872522633302</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>0.65134428167521696</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <v>85653514</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>3995</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>21</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
         <v>1.5401752190237796</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <f>32 / 12.2518055438995</f>
         <v>2.6118599324271554</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.67247386759581795</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>0.65970149253731303</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>0.65817914738445704</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>0.65885042745802802</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>85635082</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>4660</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>19</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>1.1946351931330472</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <f>32/ 15.6395952701568</f>
         <v>2.0460887540396802</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>0.67197610751617698</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>0.64228855721392997</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>0.64057131589716398</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>0.64417278042856796</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>114001930</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>5220</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>25</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>1.4032567049808429</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <f>32 /13.23637342453</f>
         <v>2.4175806298042897</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0.66998506719760997</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>0.64477611940298496</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0.64345585529285998</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>0.64487501296850602</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>85653526</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>4744</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>26</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f>C7*293/B7</f>
         <v>1.6058178752107926</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <f>32 / 11.9503273963928</f>
         <v>2.6777509049383186</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0.60328521652563405</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.59402985074626802</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>0.59245957484766099</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>0.59228914430539503</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>85616674</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>4436</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>23</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f>C8*293/B8</f>
         <v>1.5191614066726782</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <f>32 / 12.8743271827697</f>
         <v>2.4855667830802886</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>0.70084619213539001</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>0.68656716417910402</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>0.68525039116487696</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>0.68897861885716305</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>85653514</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>4619</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>24</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f>C9*293/B9</f>
         <v>1.5224074474994587</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f xml:space="preserve"> 32 / 12.6667664051055</f>
         <v>2.5262958971993039</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>0.715778994524639</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>0.68805970149253703</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>0.68660909411717697</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>0.69102997184543002</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <v>85635082</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>4661</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>19</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f t="shared" ref="D10:D12" si="1">C10*293/B10</f>
         <v>1.1943788886505042</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f xml:space="preserve"> 32 / 16.0069088935852</f>
         <v>1.999136761053476</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>0.72075659532105496</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>0.70646766169154196</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>0.70522165661944303</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>0.70676026749341603</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>113983498</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>5181</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>24</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>1.3572669368847712</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f xml:space="preserve"> 32/ 14.0491971969604</f>
         <v>2.2777102172730075</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>0.71876555500248795</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0.69253731343283498</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0.69128572810917699</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>0.69593767606894896</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>85635094</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="e">
+      <c r="B12" s="1">
+        <v>5097</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.0922111045713165</v>
+      </c>
+      <c r="E12" s="1">
+        <f>32/17.3773918151855</f>
+        <v>1.8414731244096314</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.72374315579890403</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.70447761194029801</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.70342781452877201</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.70493985269063997</v>
+      </c>
+      <c r="J12" s="1">
+        <v>113983510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit for figures
</commit_message>
<xml_diff>
--- a/models_and_metrics/metrics_summary.xlsx
+++ b/models_and_metrics/metrics_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio Coding\DL_final_project\models_and_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECFADFF-3715-4087-8C3A-F9DD6B7F8E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD108F48-6E4B-4B17-80C3-B5773E107C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32CD13F7-3551-4E15-BA67-D6630EDB706E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>EA GELU</t>
+  </si>
+  <si>
+    <t>Test Precision Change over baseline</t>
+  </si>
+  <si>
+    <t>Average Epoch time Seconds</t>
   </si>
 </sst>
 </file>
@@ -225,7 +231,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -287,7 +293,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$12</c:f>
+              <c:f>Sheet1!$H$2:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -561,7 +567,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -623,7 +629,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -897,7 +903,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -959,7 +965,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$12</c:f>
+              <c:f>Sheet1!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1233,7 +1239,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1295,7 +1301,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$12</c:f>
+              <c:f>Sheet1!$L$2:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3797,16 +3803,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4151,10 +4157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0439EB13-8DEA-4DA4-BD28-E0ABE1F425AC}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4167,10 +4173,12 @@
     <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4181,28 +4189,34 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -4213,30 +4227,37 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <f>C2*293/B2</f>
+        <f>B2/C2</f>
+        <v>189.42857142857142</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E13" si="0">C2*293/B2</f>
         <v>1.5467571644042233</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f>32 / 11.8271186351776</f>
         <v>2.7056463190300515</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.63613738178198098</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>0.60298507462686501</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>0.60112383449298201</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>0.61423096264957999</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2">
+        <v>113983510</v>
+      </c>
+      <c r="L2" s="1">
         <v>85806346</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4247,30 +4268,38 @@
         <v>21</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">C3*293/B3</f>
+        <f t="shared" ref="D3:D13" si="1">B3/C3</f>
+        <v>184.14285714285714</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>1.5911559348332041</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <f>32 / 11.816104888916</f>
         <v>2.708168241635815</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.67048282727725195</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>0.65124378109452696</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0.64995872522633302</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.65134428167521696</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3">
+        <f t="shared" ref="K3:K13" si="2">J3/0.651344281675217 - 1</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>85653514</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4281,30 +4310,38 @@
         <v>21</v>
       </c>
       <c r="D4">
+        <f t="shared" si="1"/>
+        <v>190.23809523809524</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>1.5401752190237796</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <f>32 / 12.2518055438995</f>
         <v>2.6118599324271554</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.67247386759581795</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.65970149253731303</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.65817914738445704</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.65885042745802802</v>
       </c>
-      <c r="J4">
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>1.1524083336550861E-2</v>
+      </c>
+      <c r="L4">
         <v>85635082</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -4315,30 +4352,38 @@
         <v>19</v>
       </c>
       <c r="D5">
+        <f t="shared" si="1"/>
+        <v>245.26315789473685</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>1.1946351931330472</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <f>32/ 15.6395952701568</f>
         <v>2.0460887540396802</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.67197610751617698</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.64228855721392997</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.64057131589716398</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.64417278042856796</v>
       </c>
-      <c r="J5">
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>-1.1010308140273151E-2</v>
+      </c>
+      <c r="L5">
         <v>114001930</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4349,30 +4394,38 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <f>C6*293/B6</f>
+        <f t="shared" si="1"/>
+        <v>206.8095238095238</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>1.4167626064932075</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f xml:space="preserve"> 32 / 13.2138648033142</f>
         <v>2.4216987593193782</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.65953210552513597</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.64079601990049695</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.63969087867928998</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.64025393621224402</v>
       </c>
-      <c r="J6">
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>-1.7026856264784063E-2</v>
+      </c>
+      <c r="L6">
         <v>85653526</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -4383,30 +4436,38 @@
         <v>25</v>
       </c>
       <c r="D7">
-        <f>C7*293/B7</f>
+        <f t="shared" si="1"/>
+        <v>208.8</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>1.4032567049808429</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <f>32 /13.23637342453</f>
         <v>2.4175806298042897</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.66998506719760997</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.64477611940298496</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.64345585529285998</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.64487501296850602</v>
       </c>
-      <c r="J7">
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>-9.9321800907998803E-3</v>
+      </c>
+      <c r="L7">
         <v>85653526</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -4417,30 +4478,38 @@
         <v>26</v>
       </c>
       <c r="D8">
-        <f>C8*293/B8</f>
+        <f t="shared" si="1"/>
+        <v>182.46153846153845</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>1.6058178752107926</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <f>32 / 11.9503273963928</f>
         <v>2.6777509049383186</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.60328521652563405</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.59402985074626802</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.59245957484766099</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.59228914430539503</v>
       </c>
-      <c r="J8">
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>-9.0666547678803222E-2</v>
+      </c>
+      <c r="L8">
         <v>85616674</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4451,30 +4520,38 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <f>C9*293/B9</f>
+        <f t="shared" si="1"/>
+        <v>192.86956521739131</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>1.5191614066726782</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f>32 / 12.8743271827697</f>
         <v>2.4855667830802886</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>0.70084619213539001</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>0.68656716417910402</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>0.68525039116487696</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>0.68897861885716305</v>
       </c>
-      <c r="J9">
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>5.7779485044610945E-2</v>
+      </c>
+      <c r="L9">
         <v>85653514</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -4485,30 +4562,38 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <f>C10*293/B10</f>
+        <f t="shared" si="1"/>
+        <v>192.45833333333334</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>1.5224074474994587</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f xml:space="preserve"> 32 / 12.6667664051055</f>
         <v>2.5262958971993039</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.715778994524639</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>0.68805970149253703</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>0.68660909411717697</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>0.69102997184543002</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>6.0928899334379505E-2</v>
+      </c>
+      <c r="L10" s="1">
         <v>85635082</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -4519,30 +4604,38 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D13" si="1">C11*293/B11</f>
+        <f t="shared" si="1"/>
+        <v>245.31578947368422</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>1.1943788886505042</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <f xml:space="preserve"> 32 / 16.0069088935852</f>
         <v>1.999136761053476</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.72075659532105496</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.70646766169154196</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.70522165661944303</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.70676026749341603</v>
       </c>
-      <c r="J11">
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>8.5079407891127223E-2</v>
+      </c>
+      <c r="L11">
         <v>113983498</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4554,29 +4647,37 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
+        <v>215.875</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>1.3572669368847712</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f xml:space="preserve"> 32/ 14.0491971969604</f>
         <v>2.2777102172730075</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.71876555500248795</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.69253731343283498</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.69128572810917699</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.69593767606894896</v>
       </c>
-      <c r="J12">
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>6.8463630753064386E-2</v>
+      </c>
+      <c r="L12">
         <v>85635094</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -4588,25 +4689,33 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
+        <v>268.26315789473682</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1.0922111045713165</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f>32/17.3773918151855</f>
         <v>1.8414731244096314</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>0.72374315579890403</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.70447761194029801</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.70342781452877201</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.70493985269063997</v>
       </c>
-      <c r="J13">
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>8.2284549850623501E-2</v>
+      </c>
+      <c r="L13">
         <v>113983510</v>
       </c>
     </row>

</xml_diff>